<commit_message>
delete exchange function because it doesn't work well
</commit_message>
<xml_diff>
--- a/output/ship_rule.xlsx
+++ b/output/ship_rule.xlsx
@@ -386,25 +386,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D1" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="0" t="n">
         <v>22</v>
       </c>
       <c r="F1" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G1" s="0" t="n">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I1" s="0" t="n">
-        <v>3.736020345132216</v>
+        <v>4.558084846275031</v>
       </c>
     </row>
     <row r="2">
@@ -417,25 +417,25 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>22</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>3.736020345132216</v>
+        <v>4.558084846275031</v>
       </c>
     </row>
     <row r="3">
@@ -448,25 +448,25 @@
         <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>22</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>24</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>3.736020345132216</v>
+        <v>4.558084846275031</v>
       </c>
     </row>
     <row r="4">
@@ -476,10 +476,10 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>14</v>
@@ -488,16 +488,16 @@
         <v>20</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>3.712502196630329</v>
+        <v>4.378129751786685</v>
       </c>
     </row>
     <row r="5">
@@ -507,28 +507,28 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>20</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>3.712502196630329</v>
+        <v>4.378129751786685</v>
       </c>
     </row>
     <row r="6">
@@ -538,10 +538,10 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>14</v>
@@ -550,16 +550,16 @@
         <v>20</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>3.712502196630329</v>
+        <v>4.378129751786685</v>
       </c>
     </row>
     <row r="7">
@@ -569,28 +569,28 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I7" s="0" t="n">
-        <v>3.708971512398735</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="8">
@@ -600,28 +600,28 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>3.696955406578468</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="9">
@@ -631,28 +631,28 @@
         </is>
       </c>
       <c r="B9" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>3.614318530763228</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="10">
@@ -665,25 +665,25 @@
         <v>40</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>25</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>3.614318530763228</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="11">
@@ -693,28 +693,28 @@
         </is>
       </c>
       <c r="B11" s="0" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>850</v>
+        <v>800</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>1200</v>
+        <v>1500</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>3.600891355581724</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="12">
@@ -724,28 +724,28 @@
         </is>
       </c>
       <c r="B12" s="0" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>800</v>
+        <v>2500</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>25</v>
       </c>
       <c r="I12" s="0" t="n">
-        <v>3.595854345884001</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="13">
@@ -758,25 +758,25 @@
         <v>50</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I13" s="0" t="n">
-        <v>3.595854345884001</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="14">
@@ -786,28 +786,28 @@
         </is>
       </c>
       <c r="B14" s="0" t="n">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>500</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>2000</v>
+        <v>900</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I14" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="15">
@@ -817,28 +817,28 @@
         </is>
       </c>
       <c r="B15" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="16">
@@ -848,28 +848,28 @@
         </is>
       </c>
       <c r="B16" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="C16" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="C16" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="D16" s="0" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E16" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="F16" s="0" t="n">
-        <v>800</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="I16" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="17">
@@ -882,25 +882,25 @@
         <v>10</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>800</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="18">
@@ -910,28 +910,28 @@
         </is>
       </c>
       <c r="B18" s="0" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D18" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E18" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="E18" s="0" t="n">
-        <v>21</v>
-      </c>
       <c r="F18" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="19">
@@ -941,28 +941,28 @@
         </is>
       </c>
       <c r="B19" s="0" t="n">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="E19" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="F19" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>700</v>
+        <v>1500</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="20">
@@ -972,28 +972,28 @@
         </is>
       </c>
       <c r="B20" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>600</v>
+        <v>1600</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I20" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="21">
@@ -1003,28 +1003,28 @@
         </is>
       </c>
       <c r="B21" s="0" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>1000</v>
+        <v>850</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="22">
@@ -1034,28 +1034,28 @@
         </is>
       </c>
       <c r="B22" s="0" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>1100</v>
+        <v>1400</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>1300</v>
+        <v>1600</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="23">
@@ -1068,25 +1068,25 @@
         <v>80</v>
       </c>
       <c r="C23" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D23" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>12</v>
-      </c>
       <c r="E23" s="0" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>950</v>
+        <v>500</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I23" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="24">
@@ -1096,28 +1096,28 @@
         </is>
       </c>
       <c r="B24" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>1300</v>
+        <v>700</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="25">
@@ -1127,28 +1127,28 @@
         </is>
       </c>
       <c r="B25" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="F25" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="I25" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="26">
@@ -1161,25 +1161,25 @@
         <v>30</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>1400</v>
+        <v>700</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>1500</v>
+        <v>700</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="27">
@@ -1189,28 +1189,28 @@
         </is>
       </c>
       <c r="B27" s="0" t="n">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>850</v>
+        <v>500</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="28">
@@ -1220,28 +1220,28 @@
         </is>
       </c>
       <c r="B28" s="0" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>1100</v>
+        <v>950</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>1300</v>
+        <v>2500</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>19</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="29">
@@ -1251,28 +1251,28 @@
         </is>
       </c>
       <c r="B29" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>1400</v>
+        <v>900</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="30">
@@ -1282,28 +1282,28 @@
         </is>
       </c>
       <c r="B30" s="0" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E30" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H30" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F30" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="G30" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="H30" s="0" t="n">
-        <v>17</v>
-      </c>
       <c r="I30" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="31">
@@ -1313,28 +1313,28 @@
         </is>
       </c>
       <c r="B31" s="0" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>1100</v>
+        <v>700</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>1300</v>
+        <v>700</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="32">
@@ -1344,28 +1344,28 @@
         </is>
       </c>
       <c r="B32" s="0" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="33">
@@ -1375,28 +1375,28 @@
         </is>
       </c>
       <c r="B33" s="0" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>700</v>
+        <v>2500</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>900</v>
+        <v>2500</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>13</v>
       </c>
       <c r="I33" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="34">
@@ -1406,28 +1406,28 @@
         </is>
       </c>
       <c r="B34" s="0" t="n">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>950</v>
+        <v>2500</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="35">
@@ -1437,28 +1437,28 @@
         </is>
       </c>
       <c r="B35" s="0" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="36">
@@ -1468,28 +1468,28 @@
         </is>
       </c>
       <c r="B36" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>950</v>
+        <v>1000</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="H36" s="0" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="37">
@@ -1499,28 +1499,28 @@
         </is>
       </c>
       <c r="B37" s="0" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>600</v>
+        <v>1400</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>900</v>
+        <v>1600</v>
       </c>
       <c r="H37" s="0" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="38">
@@ -1530,28 +1530,28 @@
         </is>
       </c>
       <c r="B38" s="0" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E38" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="H38" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="F38" s="0" t="n">
-        <v>900</v>
-      </c>
-      <c r="G38" s="0" t="n">
-        <v>1600</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>14</v>
-      </c>
       <c r="I38" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="39">
@@ -1561,28 +1561,28 @@
         </is>
       </c>
       <c r="B39" s="0" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>2500</v>
+        <v>1300</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="40">
@@ -1592,28 +1592,28 @@
         </is>
       </c>
       <c r="B40" s="0" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>850</v>
+        <v>1300</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>4.269132093741455</v>
       </c>
     </row>
     <row r="41">
@@ -1623,28 +1623,28 @@
         </is>
       </c>
       <c r="B41" s="0" t="n">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>1300</v>
+        <v>1400</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="42">
@@ -1654,28 +1654,28 @@
         </is>
       </c>
       <c r="B42" s="0" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>1300</v>
+        <v>900</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="43">
@@ -1685,28 +1685,28 @@
         </is>
       </c>
       <c r="B43" s="0" t="n">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>1300</v>
+        <v>850</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>1400</v>
+        <v>900</v>
       </c>
       <c r="H43" s="0" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="44">
@@ -1716,28 +1716,28 @@
         </is>
       </c>
       <c r="B44" s="0" t="n">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="45">
@@ -1747,28 +1747,28 @@
         </is>
       </c>
       <c r="B45" s="0" t="n">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>1300</v>
+        <v>2500</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>10</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="46">
@@ -1778,28 +1778,28 @@
         </is>
       </c>
       <c r="B46" s="0" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="47">
@@ -1809,28 +1809,28 @@
         </is>
       </c>
       <c r="B47" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="48">
@@ -1840,28 +1840,28 @@
         </is>
       </c>
       <c r="B48" s="0" t="n">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>600</v>
+        <v>1300</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>700</v>
+        <v>2000</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I48" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="49">
@@ -1871,28 +1871,28 @@
         </is>
       </c>
       <c r="B49" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C49" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C49" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="D49" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>950</v>
+        <v>850</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>2500</v>
+        <v>1300</v>
       </c>
       <c r="H49" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="50">
@@ -1902,28 +1902,28 @@
         </is>
       </c>
       <c r="B50" s="0" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>600</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>2000</v>
+        <v>1100</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="51">
@@ -1933,28 +1933,28 @@
         </is>
       </c>
       <c r="B51" s="0" t="n">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>850</v>
+        <v>950</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="I51" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="52">
@@ -1964,28 +1964,28 @@
         </is>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F52" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="G52" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="G52" s="0" t="n">
-        <v>2500</v>
-      </c>
       <c r="H52" s="0" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I52" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="53">
@@ -1995,28 +1995,28 @@
         </is>
       </c>
       <c r="B53" s="0" t="n">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>19</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G53" s="0" t="n">
-        <v>2500</v>
+        <v>950</v>
       </c>
       <c r="H53" s="0" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I53" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="54">
@@ -2026,28 +2026,28 @@
         </is>
       </c>
       <c r="B54" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>1300</v>
+        <v>1600</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I54" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="55">
@@ -2057,28 +2057,28 @@
         </is>
       </c>
       <c r="B55" s="0" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>140</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>850</v>
+        <v>2500</v>
       </c>
       <c r="H55" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I55" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="56">
@@ -2091,25 +2091,25 @@
         <v>40</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>700</v>
+        <v>1600</v>
       </c>
       <c r="G56" s="0" t="n">
-        <v>800</v>
+        <v>2500</v>
       </c>
       <c r="H56" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I56" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="57">
@@ -2119,28 +2119,28 @@
         </is>
       </c>
       <c r="B57" s="0" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>850</v>
+        <v>1300</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I57" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="58">
@@ -2150,28 +2150,28 @@
         </is>
       </c>
       <c r="B58" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C58" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="C58" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="D58" s="0" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>850</v>
+        <v>600</v>
       </c>
       <c r="G58" s="0" t="n">
-        <v>2500</v>
+        <v>800</v>
       </c>
       <c r="H58" s="0" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I58" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="59">
@@ -2181,28 +2181,28 @@
         </is>
       </c>
       <c r="B59" s="0" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="C59" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D59" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D59" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="E59" s="0" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F59" s="0" t="n">
+        <v>900</v>
+      </c>
+      <c r="G59" s="0" t="n">
         <v>1200</v>
       </c>
-      <c r="G59" s="0" t="n">
-        <v>1300</v>
-      </c>
       <c r="H59" s="0" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I59" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="60">
@@ -2212,28 +2212,28 @@
         </is>
       </c>
       <c r="B60" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="G60" s="0" t="n">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I60" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="61">
@@ -2243,28 +2243,28 @@
         </is>
       </c>
       <c r="B61" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I61" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="62">
@@ -2274,19 +2274,19 @@
         </is>
       </c>
       <c r="B62" s="0" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>950</v>
+        <v>1300</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>2500</v>
@@ -2295,7 +2295,7 @@
         <v>12</v>
       </c>
       <c r="I62" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="63">
@@ -2305,28 +2305,28 @@
         </is>
       </c>
       <c r="B63" s="0" t="n">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D63" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E63" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="E63" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="F63" s="0" t="n">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="H63" s="0" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I63" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="64">
@@ -2336,28 +2336,28 @@
         </is>
       </c>
       <c r="B64" s="0" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>850</v>
+        <v>1400</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>2500</v>
       </c>
       <c r="H64" s="0" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I64" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="65">
@@ -2367,28 +2367,28 @@
         </is>
       </c>
       <c r="B65" s="0" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E65" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="H65" s="0" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I65" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="66">
@@ -2401,25 +2401,25 @@
         <v>130</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E66" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="H66" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="F66" s="0" t="n">
-        <v>850</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H66" s="0" t="n">
-        <v>17</v>
-      </c>
       <c r="I66" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="67">
@@ -2429,28 +2429,28 @@
         </is>
       </c>
       <c r="B67" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C67" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C67" s="0" t="n">
-        <v>60</v>
-      </c>
       <c r="D67" s="0" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I67" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="68">
@@ -2460,28 +2460,28 @@
         </is>
       </c>
       <c r="B68" s="0" t="n">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>850</v>
+        <v>1300</v>
       </c>
       <c r="G68" s="0" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="H68" s="0" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I68" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="69">
@@ -2491,28 +2491,28 @@
         </is>
       </c>
       <c r="B69" s="0" t="n">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="G69" s="0" t="n">
         <v>1300</v>
       </c>
       <c r="H69" s="0" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I69" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="70">
@@ -2522,28 +2522,28 @@
         </is>
       </c>
       <c r="B70" s="0" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>900</v>
+        <v>1600</v>
       </c>
       <c r="H70" s="0" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I70" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="71">
@@ -2553,28 +2553,28 @@
         </is>
       </c>
       <c r="B71" s="0" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>1400</v>
+        <v>700</v>
       </c>
       <c r="G71" s="0" t="n">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I71" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="72">
@@ -2584,28 +2584,28 @@
         </is>
       </c>
       <c r="B72" s="0" t="n">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>950</v>
+        <v>500</v>
       </c>
       <c r="G72" s="0" t="n">
-        <v>2500</v>
+        <v>1200</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I72" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="73">
@@ -2615,28 +2615,28 @@
         </is>
       </c>
       <c r="B73" s="0" t="n">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="G73" s="0" t="n">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I73" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="74">
@@ -2646,28 +2646,28 @@
         </is>
       </c>
       <c r="B74" s="0" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E74" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="G74" s="0" t="n">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I74" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="75">
@@ -2680,25 +2680,25 @@
         <v>30</v>
       </c>
       <c r="C75" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D75" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D75" s="0" t="n">
-        <v>25</v>
-      </c>
       <c r="E75" s="0" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="G75" s="0" t="n">
         <v>2500</v>
       </c>
       <c r="H75" s="0" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I75" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="76">
@@ -2708,28 +2708,28 @@
         </is>
       </c>
       <c r="B76" s="0" t="n">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F76" s="0" t="n">
         <v>500</v>
       </c>
       <c r="G76" s="0" t="n">
-        <v>950</v>
+        <v>1500</v>
       </c>
       <c r="H76" s="0" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I76" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="77">
@@ -2739,28 +2739,28 @@
         </is>
       </c>
       <c r="B77" s="0" t="n">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="G77" s="0" t="n">
-        <v>1300</v>
+        <v>1600</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I77" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="78">
@@ -2770,28 +2770,28 @@
         </is>
       </c>
       <c r="B78" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="G78" s="0" t="n">
-        <v>1400</v>
+        <v>1100</v>
       </c>
       <c r="H78" s="0" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I78" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="79">
@@ -2801,28 +2801,28 @@
         </is>
       </c>
       <c r="B79" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E79" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="G79" s="0" t="n">
-        <v>2500</v>
+        <v>850</v>
       </c>
       <c r="H79" s="0" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I79" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="80">
@@ -2832,28 +2832,28 @@
         </is>
       </c>
       <c r="B80" s="0" t="n">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D80" s="0" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E80" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="G80" s="0" t="n">
-        <v>1100</v>
+        <v>2000</v>
       </c>
       <c r="H80" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I80" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="81">
@@ -2863,28 +2863,28 @@
         </is>
       </c>
       <c r="B81" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E81" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="H81" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="F81" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="G81" s="0" t="n">
-        <v>1400</v>
-      </c>
-      <c r="H81" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="I81" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="82">
@@ -2894,28 +2894,28 @@
         </is>
       </c>
       <c r="B82" s="0" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E82" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>800</v>
+        <v>1500</v>
       </c>
       <c r="G82" s="0" t="n">
-        <v>800</v>
+        <v>2500</v>
       </c>
       <c r="H82" s="0" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I82" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="83">
@@ -2925,28 +2925,28 @@
         </is>
       </c>
       <c r="B83" s="0" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D83" s="0" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E83" s="0" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="G83" s="0" t="n">
-        <v>1400</v>
+        <v>2000</v>
       </c>
       <c r="H83" s="0" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I83" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="84">
@@ -2959,7 +2959,7 @@
         <v>80</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>14</v>
@@ -2968,16 +2968,16 @@
         <v>21</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>1300</v>
+        <v>950</v>
       </c>
       <c r="G84" s="0" t="n">
-        <v>1600</v>
+        <v>950</v>
       </c>
       <c r="H84" s="0" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I84" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="85">
@@ -2987,28 +2987,28 @@
         </is>
       </c>
       <c r="B85" s="0" t="n">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="D85" s="0" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E85" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="G85" s="0" t="n">
-        <v>700</v>
+        <v>1200</v>
       </c>
       <c r="H85" s="0" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I85" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="86">
@@ -3018,28 +3018,28 @@
         </is>
       </c>
       <c r="B86" s="0" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E86" s="0" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>1000</v>
+        <v>1400</v>
       </c>
       <c r="G86" s="0" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="H86" s="0" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I86" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="87">
@@ -3049,28 +3049,28 @@
         </is>
       </c>
       <c r="B87" s="0" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>12</v>
       </c>
       <c r="E87" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>1400</v>
+        <v>600</v>
       </c>
       <c r="G87" s="0" t="n">
-        <v>1500</v>
+        <v>2500</v>
       </c>
       <c r="H87" s="0" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I87" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="88">
@@ -3080,28 +3080,28 @@
         </is>
       </c>
       <c r="B88" s="0" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E88" s="0" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="G88" s="0" t="n">
-        <v>950</v>
+        <v>800</v>
       </c>
       <c r="H88" s="0" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I88" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="89">
@@ -3111,28 +3111,28 @@
         </is>
       </c>
       <c r="B89" s="0" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E89" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H89" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="F89" s="0" t="n">
-        <v>900</v>
-      </c>
-      <c r="G89" s="0" t="n">
-        <v>1400</v>
-      </c>
-      <c r="H89" s="0" t="n">
-        <v>21</v>
-      </c>
       <c r="I89" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="90">
@@ -3142,28 +3142,28 @@
         </is>
       </c>
       <c r="B90" s="0" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>110</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E90" s="0" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="G90" s="0" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="H90" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I90" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="91">
@@ -3173,28 +3173,28 @@
         </is>
       </c>
       <c r="B91" s="0" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D91" s="0" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E91" s="0" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F91" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="G91" s="0" t="n">
         <v>950</v>
-      </c>
-      <c r="G91" s="0" t="n">
-        <v>1600</v>
       </c>
       <c r="H91" s="0" t="n">
         <v>17</v>
       </c>
       <c r="I91" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="92">
@@ -3204,28 +3204,28 @@
         </is>
       </c>
       <c r="B92" s="0" t="n">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E92" s="0" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="G92" s="0" t="n">
-        <v>1400</v>
+        <v>1200</v>
       </c>
       <c r="H92" s="0" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I92" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="93">
@@ -3235,28 +3235,28 @@
         </is>
       </c>
       <c r="B93" s="0" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D93" s="0" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E93" s="0" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="G93" s="0" t="n">
-        <v>950</v>
+        <v>1400</v>
       </c>
       <c r="H93" s="0" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I93" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="94">
@@ -3266,28 +3266,28 @@
         </is>
       </c>
       <c r="B94" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C94" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="C94" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="D94" s="0" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E94" s="0" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="G94" s="0" t="n">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="H94" s="0" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I94" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="95">
@@ -3297,28 +3297,28 @@
         </is>
       </c>
       <c r="B95" s="0" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D95" s="0" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E95" s="0" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>1300</v>
+        <v>500</v>
       </c>
       <c r="G95" s="0" t="n">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="H95" s="0" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I95" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="96">
@@ -3328,28 +3328,28 @@
         </is>
       </c>
       <c r="B96" s="0" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E96" s="0" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="G96" s="0" t="n">
-        <v>700</v>
+        <v>1600</v>
       </c>
       <c r="H96" s="0" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I96" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="97">
@@ -3359,28 +3359,28 @@
         </is>
       </c>
       <c r="B97" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E97" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C97" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D97" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E97" s="0" t="n">
-        <v>17</v>
-      </c>
       <c r="F97" s="0" t="n">
-        <v>1300</v>
+        <v>600</v>
       </c>
       <c r="G97" s="0" t="n">
-        <v>1400</v>
+        <v>800</v>
       </c>
       <c r="H97" s="0" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I97" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="98">
@@ -3390,28 +3390,28 @@
         </is>
       </c>
       <c r="B98" s="0" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E98" s="0" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>950</v>
+        <v>500</v>
       </c>
       <c r="G98" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
       <c r="H98" s="0" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="I98" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="99">
@@ -3421,28 +3421,28 @@
         </is>
       </c>
       <c r="B99" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E99" s="0" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="G99" s="0" t="n">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="H99" s="0" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I99" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="100">
@@ -3452,28 +3452,28 @@
         </is>
       </c>
       <c r="B100" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C100" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C100" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="D100" s="0" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E100" s="0" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>850</v>
+        <v>600</v>
       </c>
       <c r="G100" s="0" t="n">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="H100" s="0" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I100" s="0" t="n">
-        <v>3.591913341280337</v>
+        <v>3.671173135269061</v>
       </c>
     </row>
     <row r="101">

</xml_diff>